<commit_message>
updated Linked List code
updated Linked List code
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestData.xlsx
+++ b/src/test/resources/Excel/TestData.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lavanya Yelakala\eclipse-workspace\DSAlgo_TeamAchievers\src\test\resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lavanya Yelakala\eclipse-workspace\testng_dsAlgo\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D16A0C5-0006-4D51-A537-DD7F00EDBC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E3D4EB-E41E-41C9-9FDB-8BF24B13FF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="2" r:id="rId1"/>
-    <sheet name="login1" sheetId="3" r:id="rId2"/>
-    <sheet name="login" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
-    <sheet name="pythonCode1" sheetId="4" r:id="rId5"/>
-    <sheet name="tryEditorCode" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="pythonCode1" sheetId="4" r:id="rId3"/>
+    <sheet name="tryEditorCode2" sheetId="7" r:id="rId4"/>
+    <sheet name="tryEditorCode" sheetId="9" r:id="rId5"/>
+    <sheet name="Login" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
   <si>
     <t>username</t>
   </si>
@@ -75,49 +75,10 @@
   </si>
   <si>
     <t xml:space="preserve"> fcbhgug5mkji</t>
-  </si>
-  <si>
-    <t>konikd356</t>
-  </si>
-  <si>
-    <t>lilataghn451</t>
-  </si>
-  <si>
-    <t>janogsd39</t>
-  </si>
-  <si>
-    <t>xersrtdfokokjuhgyh673</t>
-  </si>
-  <si>
-    <t>xswsedrfc589cff</t>
-  </si>
-  <si>
-    <t>bhvgfgfyhu123</t>
   </si>
   <si>
     <t>Feature File
 scenario number</t>
-  </si>
-  <si>
-    <t>testtttt</t>
-  </si>
-  <si>
-    <t>testttt</t>
-  </si>
-  <si>
-    <t>ytyutu</t>
-  </si>
-  <si>
-    <t>qachamps3</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Ninjatest@123</t>
-  </si>
-  <si>
-    <t>abc</t>
   </si>
   <si>
     <t>pythonCode</t>
@@ -262,9 +223,6 @@
     <t>Welcome@25!</t>
   </si>
   <si>
-    <t>Verify that user receives error message for all empty fields during Login</t>
-  </si>
-  <si>
     <t>errorMsg</t>
   </si>
   <si>
@@ -274,12 +232,6 @@
     <t>Password12</t>
   </si>
   <si>
-    <t>Verify that user receives error message for empty Username field during Login</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Username25</t>
   </si>
   <si>
@@ -301,9 +253,6 @@
     <t>USer9999569</t>
   </si>
   <si>
-    <t>Verify that user receives error message for empty Password field during Login</t>
-  </si>
-  <si>
     <t>Verify that user receives error message for invalid Username and invalid Password fields during Login</t>
   </si>
   <si>
@@ -347,27 +296,46 @@
   </si>
   <si>
     <t>gdfgdgdfhdhd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectedAlertMessage                </t>
+  </si>
+  <si>
+    <t>scenario identifier</t>
+  </si>
+  <si>
+    <t>Invalid Username and Password</t>
+  </si>
+  <si>
+    <t>You are logged in</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+    squares_list = []
+    for i in range(len(nums)):
+        square = nums[i] * nums[i]
+        squares_list.append(square)
+    sorted_squares_list = sorted(squares_list)
+    print(sorted_squares_list)
+    return sorted_squares_list
+# Example usage
+sortedSquares([-7, -3, 2, 3, 11])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid code </t>
+  </si>
+  <si>
+    <t>valid code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,7 +417,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -460,26 +428,30 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -844,20 +816,20 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="D2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1">
@@ -866,9 +838,9 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="1">
@@ -877,12 +849,12 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="1">
@@ -891,7 +863,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -899,7 +871,7 @@
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="1">
@@ -908,15 +880,15 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="1">
@@ -925,15 +897,15 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="1">
@@ -942,16 +914,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>50</v>
+        <v>31</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="F8" s="1">
         <v>6</v>
@@ -959,15 +931,15 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="1">
@@ -976,15 +948,15 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="1">
@@ -993,15 +965,15 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="1">
@@ -1014,87 +986,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5AF72C-2997-422C-89B0-2C3C703E5609}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351C18B5-3A3C-4F9E-AE6C-5DBDCA23E4ED}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>15</v>
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>17</v>
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>54</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1103,204 +1057,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF4F130-7460-44A6-A612-2786A37CAEED}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="82" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="48.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="C2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351C18B5-3A3C-4F9E-AE6C-5DBDCA23E4ED}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C1BB72-E077-4E53-9B8E-2362A02F5343}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1311,75 +1072,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>30</v>
+      <c r="A1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="172.8">
-      <c r="A2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>31</v>
+      <c r="A2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="172.8">
-      <c r="A3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>38</v>
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="273.60000000000002">
-      <c r="A4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>32</v>
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="273.60000000000002">
-      <c r="A5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>38</v>
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="201.6">
-      <c r="A6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>32</v>
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="201.6">
-      <c r="A7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>39</v>
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="158.4">
-      <c r="A8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>33</v>
+      <c r="A8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="158.4">
-      <c r="A9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>40</v>
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF521D5E-4550-427D-AF53-CC1823D613EE}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15" thickBot="1">
+      <c r="A1" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" thickBot="1">
+      <c r="A2" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15" thickBot="1">
+      <c r="A3" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2E2688-978F-4CA4-B38E-2E63FEA1C3A4}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="47" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" customHeight="1" thickBot="1">
+      <c r="A1" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="172.8">
+      <c r="A2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="172.8">
+      <c r="A3" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1388,31 +1220,123 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF521D5E-4550-427D-AF53-CC1823D613EE}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922B8DA6-F91A-4735-900F-38E328F7A407}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" thickBot="1">
-      <c r="A1" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="15" thickBot="1">
-      <c r="A2" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15" thickBot="1">
-      <c r="A3" s="14" t="s">
-        <v>87</v>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>